<commit_message>
Added modifications to regional
</commit_message>
<xml_diff>
--- a/src/Shapefile_prep/shapefile_settings.xlsx
+++ b/src/Shapefile_prep/shapefile_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafal\Downloads\MRAT GIT\MRAT GIT\src\Shapefile_prep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f5aee5c5b004427f/Documents/mr-risk-assessment-regional/src/Shapefile_prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4718E78-D645-44DF-8C7A-677055DD56F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{D4718E78-D645-44DF-8C7A-677055DD56F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6B2BB74-7ECB-4573-A807-64A48CF55A3F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9BCEFF0F-9A23-954A-B88D-C463C9BBC742}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9BCEFF0F-9A23-954A-B88D-C463C9BBC742}"/>
   </bookViews>
   <sheets>
     <sheet name="SETTINGS" sheetId="2" r:id="rId1"/>
@@ -65,22 +65,22 @@
     <t>ADMIN1 ID</t>
   </si>
   <si>
-    <t>JSON</t>
-  </si>
-  <si>
-    <t>Belize_districts_GeoJSON</t>
-  </si>
-  <si>
-    <t>ADMIN1_ID</t>
-  </si>
-  <si>
-    <t>ADMIN1_NAM</t>
-  </si>
-  <si>
-    <t>ADMIN2_ID</t>
-  </si>
-  <si>
-    <t>ADMIN2_NAM</t>
+    <t>CTRY_ISO_N</t>
+  </si>
+  <si>
+    <t>REGION_C</t>
+  </si>
+  <si>
+    <t>CTRY_ISOA3</t>
+  </si>
+  <si>
+    <t>SHP</t>
+  </si>
+  <si>
+    <t>amro_simplified</t>
+  </si>
+  <si>
+    <t>REGION_N</t>
   </si>
 </sst>
 </file>
@@ -527,79 +527,79 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="161" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="161" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.19921875" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.296875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="10.796875" style="1"/>
+    <col min="1" max="1" width="17.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.33203125" style="4" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="7" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="25.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="26" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>

</xml_diff>